<commit_message>
update code tao report
</commit_message>
<xml_diff>
--- a/Ver2/Notion data/Chấm công HỆ THỐNG.xlsx
+++ b/Ver2/Notion data/Chấm công HỆ THỐNG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AQ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,17 +658,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>44a59162-be99-4049-96cd-2374839aa086</t>
+          <t>3591e46b-a1b0-448e-a0a6-afcd443b310e</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-08T16:49:00.000Z</t>
+          <t>2024-07-24T15:30:00.000Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.notion.so/44a59162be99404996cd2374839aa086</t>
+          <t>https://www.notion.so/3591e46ba1b0448ea0a6afcd443b310e</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -753,7 +753,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>[{'id': 'ea0572af-f8c9-430d-9d95-23303a4ce4cd'}]</t>
+          <t>[{'id': '35f44955-2223-488a-8274-8db6f726d9f7'}]</t>
         </is>
       </c>
       <c r="Z2" t="b">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
@@ -847,17 +847,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>39c98d7f-b7d0-49ef-9652-f406a3e62029</t>
+          <t>29f35f86-976a-4c89-9a70-f1c1f07bcf2a</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-07-08T16:48:00.000Z</t>
+          <t>2024-07-24T15:30:00.000Z</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -870,7 +870,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://www.notion.so/39c98d7fb7d049ef9652f406a3e62029</t>
+          <t>https://www.notion.so/29f35f86976a4c899a70f1c1f07bcf2a</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -942,7 +942,7 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>[{'id': 'e0ac0375-0b3a-4c88-a613-cb8df33ebe6b'}]</t>
+          <t>[{'id': '3db76400-46c0-4adb-9d9c-51542f2de2f9'}]</t>
         </is>
       </c>
       <c r="Z3" t="b">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="AF3" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4a76f2d2-b0f3-4746-8b60-6095030ce9a4</t>
+          <t>44a59162-be99-4049-96cd-2374839aa086</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-07-08T16:48:00.000Z</t>
+          <t>2024-07-08T16:49:00.000Z</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.notion.so/4a76f2d2b0f347468b606095030ce9a4</t>
+          <t>https://www.notion.so/44a59162be99404996cd2374839aa086</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>[{'id': '90bc02c2-bd1e-4c33-884a-38a1db528c78'}]</t>
+          <t>[{'id': 'ea0572af-f8c9-430d-9d95-23303a4ce4cd'}]</t>
         </is>
       </c>
       <c r="Z4" t="b">
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="AF4" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr">
@@ -1225,17 +1225,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8e8f7e77-65ea-4667-9635-359ff100cf58</t>
+          <t>39c98d7f-b7d0-49ef-9652-f406a3e62029</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-07-08T16:47:00.000Z</t>
+          <t>2024-07-08T16:48:00.000Z</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.notion.so/8e8f7e7765ea46679635359ff100cf58</t>
+          <t>https://www.notion.so/39c98d7fb7d049ef9652f406a3e62029</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>[{'id': '6454d5e5-8a20-473b-a597-dc1973dd1e0e'}]</t>
+          <t>[{'id': 'e0ac0375-0b3a-4c88-a613-cb8df33ebe6b'}]</t>
         </is>
       </c>
       <c r="Z5" t="b">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
@@ -1414,17 +1414,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0326afbb-4995-4ae7-8b30-901ef3dd038c</t>
+          <t>4a76f2d2-b0f3-4746-8b60-6095030ce9a4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-07-08T16:45:00.000Z</t>
+          <t>2024-07-08T16:48:00.000Z</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.notion.so/0326afbb49954ae78b30901ef3dd038c</t>
+          <t>https://www.notion.so/4a76f2d2b0f347468b606095030ce9a4</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>[{'id': 'bc9b2b6b-3140-44b9-a1be-4dc8e77d8898'}]</t>
+          <t>[{'id': '90bc02c2-bd1e-4c33-884a-38a1db528c78'}]</t>
         </is>
       </c>
       <c r="Z6" t="b">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="AF6" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
@@ -1603,17 +1603,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8170c5f7-1afc-4ec2-b5bf-4dfa06dfd8a8</t>
+          <t>8e8f7e77-65ea-4667-9635-359ff100cf58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-07-08T16:45:00.000Z</t>
+          <t>2024-07-08T16:47:00.000Z</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.notion.so/8170c5f71afc4ec2b5bf4dfa06dfd8a8</t>
+          <t>https://www.notion.so/8e8f7e7765ea46679635359ff100cf58</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>[{'id': '7e29a9ca-b017-4ad6-a6b0-6ed9330137bc'}]</t>
+          <t>[{'id': '6454d5e5-8a20-473b-a597-dc1973dd1e0e'}]</t>
         </is>
       </c>
       <c r="Z7" t="b">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="AF7" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
@@ -1792,17 +1792,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0f6b9d94-3550-435e-9360-d1dd8933363f</t>
+          <t>0326afbb-4995-4ae7-8b30-901ef3dd038c</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-07-06T10:33:00.000Z</t>
+          <t>2024-07-08T16:45:00.000Z</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.notion.so/0f6b9d943550435e9360d1dd8933363f</t>
+          <t>https://www.notion.so/0326afbb49954ae78b30901ef3dd038c</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>[{'id': 'd8178da7-a5cc-474f-9c6e-ed3029f89c4d'}]</t>
+          <t>[{'id': 'bc9b2b6b-3140-44b9-a1be-4dc8e77d8898'}]</t>
         </is>
       </c>
       <c r="Z8" t="b">
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="AF8" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="AI8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
@@ -1981,17 +1981,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05de003a-828f-46b1-ba9c-63df15fb2410</t>
+          <t>8170c5f7-1afc-4ec2-b5bf-4dfa06dfd8a8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:45:00.000Z</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.notion.so/05de003a828f46b1ba9c63df15fb2410</t>
+          <t>https://www.notion.so/8170c5f71afc4ec2b5bf4dfa06dfd8a8</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>[{'id': 'f973382b-037a-4eb1-84bc-e9e5318184b8'}]</t>
+          <t>[{'id': '7e29a9ca-b017-4ad6-a6b0-6ed9330137bc'}]</t>
         </is>
       </c>
       <c r="Z9" t="b">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="AF9" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="AI9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
@@ -2170,17 +2170,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1cf1ba2b-e08a-4452-b208-684506d74f54</t>
+          <t>0f6b9d94-3550-435e-9360-d1dd8933363f</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-06T10:33:00.000Z</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.notion.so/1cf1ba2be08a4452b208684506d74f54</t>
+          <t>https://www.notion.so/0f6b9d943550435e9360d1dd8933363f</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>[{'id': '3fac4a49-402c-4d34-aa91-419ebc20760c'}]</t>
+          <t>[{'id': 'd8178da7-a5cc-474f-9c6e-ed3029f89c4d'}]</t>
         </is>
       </c>
       <c r="Z10" t="b">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="AF10" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG10" t="inlineStr">
         <is>
@@ -2308,7 +2308,7 @@
         </is>
       </c>
       <c r="AI10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
       <c r="AN10" t="inlineStr">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>dda0b264-3b1d-46ab-85d8-06a4ac6fc467</t>
+          <t>05de003a-828f-46b1-ba9c-63df15fb2410</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.notion.so/dda0b2643b1d46ab85d806a4ac6fc467</t>
+          <t>https://www.notion.so/05de003a828f46b1ba9c63df15fb2410</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="S11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>[{'id': '75046948-a198-4627-89b3-3bbf5967526b'}]</t>
+          <t>[{'id': 'f973382b-037a-4eb1-84bc-e9e5318184b8'}]</t>
         </is>
       </c>
       <c r="Z11" t="b">
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="AF11" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>36015951-56f5-48c6-b457-456fdded4f32</t>
+          <t>1cf1ba2b-e08a-4452-b208-684506d74f54</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.notion.so/3601595156f548c6b457456fdded4f32</t>
+          <t>https://www.notion.so/1cf1ba2be08a4452b208684506d74f54</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>[{'id': 'e49d0ce3-124d-4e4b-b377-be2139cde3f5'}]</t>
+          <t>[{'id': '3fac4a49-402c-4d34-aa91-419ebc20760c'}]</t>
         </is>
       </c>
       <c r="Z12" t="b">
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="AF12" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="AI12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN12" t="inlineStr">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>48a1d5d5-449f-4119-b338-1f7d4ea3464f</t>
+          <t>dda0b264-3b1d-46ab-85d8-06a4ac6fc467</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.notion.so/48a1d5d5449f4119b3381f7d4ea3464f</t>
+          <t>https://www.notion.so/dda0b2643b1d46ab85d806a4ac6fc467</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="S13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>[{'id': 'c463b1a9-4fb2-4258-87a7-44193ba02405'}]</t>
+          <t>[{'id': '75046948-a198-4627-89b3-3bbf5967526b'}]</t>
         </is>
       </c>
       <c r="Z13" t="b">
@@ -2849,7 +2849,7 @@
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="AF13" t="n">
-        <v>17</v>
+        <v>27.5</v>
       </c>
       <c r="AG13" t="inlineStr">
         <is>
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="AI13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" t="inlineStr">
         <is>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="AM13" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN13" t="inlineStr">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4a2d1406-11a9-4e3c-80ff-0b01e9355c9b</t>
+          <t>36015951-56f5-48c6-b457-456fdded4f32</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.notion.so/4a2d140611a94e3c80ff0b01e9355c9b</t>
+          <t>https://www.notion.so/3601595156f548c6b457456fdded4f32</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="S14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>[{'id': 'e926d62c-e624-4663-9009-c562ae5166cf'}]</t>
+          <t>[{'id': 'e49d0ce3-124d-4e4b-b377-be2139cde3f5'}]</t>
         </is>
       </c>
       <c r="Z14" t="b">
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="AF14" t="n">
-        <v>22.5</v>
+        <v>24</v>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
@@ -3064,7 +3064,7 @@
         </is>
       </c>
       <c r="AI14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ14" t="inlineStr">
         <is>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN14" t="inlineStr">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>71bb8625-d14d-41b5-8a04-475b11876eae</t>
+          <t>48a1d5d5-449f-4119-b338-1f7d4ea3464f</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.notion.so/71bb8625d14d41b58a04475b11876eae</t>
+          <t>https://www.notion.so/48a1d5d5449f4119b3381f7d4ea3464f</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -3183,7 +3183,7 @@
         </is>
       </c>
       <c r="S15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="V15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" t="inlineStr">
         <is>
@@ -3210,7 +3210,7 @@
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>[{'id': '3d301dfe-6e3d-4d28-a249-1fd5fac9abd3'}]</t>
+          <t>[{'id': 'c463b1a9-4fb2-4258-87a7-44193ba02405'}]</t>
         </is>
       </c>
       <c r="Z15" t="b">
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="AF15" t="n">
-        <v>18.5</v>
+        <v>20</v>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>82923c0d-8cf4-4fa1-a3b5-52255c0fbc91</t>
+          <t>4a2d1406-11a9-4e3c-80ff-0b01e9355c9b</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.notion.so/82923c0d8cf44fa1a3b552255c0fbc91</t>
+          <t>https://www.notion.so/4a2d140611a94e3c80ff0b01e9355c9b</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="S16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>[{'id': 'a73ea60d-3de1-4e9b-aa7b-f22fda5742bd'}]</t>
+          <t>[{'id': 'e926d62c-e624-4663-9009-c562ae5166cf'}]</t>
         </is>
       </c>
       <c r="Z16" t="b">
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
@@ -3429,7 +3429,7 @@
         </is>
       </c>
       <c r="AF16" t="n">
-        <v>20</v>
+        <v>23.5</v>
       </c>
       <c r="AG16" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="AI16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ16" t="inlineStr">
         <is>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="AM16" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
       <c r="AN16" t="inlineStr">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8838c6b8-138d-4a51-b94c-a61e43096f82</t>
+          <t>71bb8625-d14d-41b5-8a04-475b11876eae</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://www.notion.so/8838c6b8138d4a51b94ca61e43096f82</t>
+          <t>https://www.notion.so/71bb8625d14d41b58a04475b11876eae</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -3561,21 +3561,21 @@
         </is>
       </c>
       <c r="S17" t="n">
+        <v>3</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
         <v>1</v>
       </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>%3CK%3FH</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
       <c r="W17" t="inlineStr">
         <is>
           <t>Kfrh</t>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>[{'id': '3601e7b0-a80d-4dfd-bfa1-0d34a0e7e389'}]</t>
+          <t>[{'id': '3d301dfe-6e3d-4d28-a249-1fd5fac9abd3'}]</t>
         </is>
       </c>
       <c r="Z17" t="b">
@@ -3605,7 +3605,7 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="AF17" t="n">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="AM17" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN17" t="inlineStr">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ce5aa8e2-193e-4cfb-85c8-d1f2bb956fbc</t>
+          <t>82923c0d-8cf4-4fa1-a3b5-52255c0fbc91</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://www.notion.so/ce5aa8e2193e4cfb85c8d1f2bb956fbc</t>
+          <t>https://www.notion.so/82923c0d8cf44fa1a3b552255c0fbc91</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -3763,7 +3763,7 @@
         </is>
       </c>
       <c r="V18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W18" t="inlineStr">
         <is>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>[{'id': 'b9c67786-5d99-45c1-85d7-f96bfb66ef22'}]</t>
+          <t>[{'id': 'a73ea60d-3de1-4e9b-aa7b-f22fda5742bd'}]</t>
         </is>
       </c>
       <c r="Z18" t="b">
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
@@ -3820,7 +3820,7 @@
         </is>
       </c>
       <c r="AI18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ18" t="inlineStr">
         <is>
@@ -3871,7 +3871,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>d482bb7f-6b24-4f14-958b-0282197809bf</t>
+          <t>8838c6b8-138d-4a51-b94c-a61e43096f82</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://www.notion.so/d482bb7f6b244f14958b0282197809bf</t>
+          <t>https://www.notion.so/8838c6b8138d4a51b94ca61e43096f82</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>[{'id': '467f676f-8f46-49b5-afea-feecb0794d23'}]</t>
+          <t>[{'id': '3601e7b0-a80d-4dfd-bfa1-0d34a0e7e389'}]</t>
         </is>
       </c>
       <c r="Z19" t="b">
@@ -3983,7 +3983,7 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="AF19" t="n">
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="AG19" t="inlineStr">
         <is>
@@ -4009,7 +4009,7 @@
         </is>
       </c>
       <c r="AI19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ19" t="inlineStr">
         <is>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>f16ce82e-4786-421e-a21c-3d6a57cbc51d</t>
+          <t>ce5aa8e2-193e-4cfb-85c8-d1f2bb956fbc</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-23T18:58:00.000Z</t>
+          <t>2024-07-24T16:01:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://www.notion.so/f16ce82e4786421ea21c3d6a57cbc51d</t>
+          <t>https://www.notion.so/ce5aa8e2193e4cfb85c8d1f2bb956fbc</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -4155,87 +4155,465 @@
       </c>
       <c r="Y20" t="inlineStr">
         <is>
+          <t>[{'id': 'b9c67786-5d99-45c1-85d7-f96bfb66ef22'}]</t>
+        </is>
+      </c>
+      <c r="Z20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC20" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF20" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+        </is>
+      </c>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP20" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>d482bb7f-6b24-4f14-958b-0282197809bf</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2024-07-24T16:01:00.000Z</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/d482bb7f6b244f14958b0282197809bf</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>[{'id': '467f676f-8f46-49b5-afea-feecb0794d23'}]</t>
+        </is>
+      </c>
+      <c r="Z21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC21" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF21" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH21" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM21" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+        </is>
+      </c>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO21" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP21" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>f16ce82e-4786-421e-a21c-3d6a57cbc51d</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2024-07-24T16:01:00.000Z</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/f16ce82e4786421ea21c3d6a57cbc51d</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
           <t>[{'id': 'd1ae645f-f3dd-46cd-a715-a8c150605da6'}]</t>
         </is>
       </c>
-      <c r="Z20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA20" t="inlineStr">
+      <c r="Z22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="inlineStr">
         <is>
           <t>avzr</t>
         </is>
       </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AC20" t="n">
-        <v>23</v>
-      </c>
-      <c r="AD20" t="inlineStr">
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD22" t="inlineStr">
         <is>
           <t>rCIq</t>
         </is>
       </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AF20" t="n">
-        <v>23</v>
-      </c>
-      <c r="AG20" t="inlineStr">
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF22" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG22" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="AH20" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AI20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ20" t="inlineStr">
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="AK20" t="inlineStr">
+      <c r="AK22" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="AL20" t="inlineStr">
+      <c r="AL22" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="AM20" t="inlineStr">
+      <c r="AM22" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="AN20" t="inlineStr">
+      <c r="AN22" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="AO20" t="inlineStr">
+      <c r="AO22" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AP20" t="inlineStr">
+      <c r="AP22" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AQ20" t="inlineStr">
+      <c r="AQ22" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>